<commit_message>
layout changes stakeholder analysis
</commit_message>
<xml_diff>
--- a/stakeholder analysis.xlsx
+++ b/stakeholder analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nourb\Documents\Semester 4\IS Project Management\übungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nourb\Documents\GitHub\ProjM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7A5BAC-8ECE-4356-A2D6-3B05E59D6228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB6671-A7EA-44E8-87C5-601EC0AE258B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stakeholder Analysis" sheetId="1" r:id="rId1"/>
@@ -273,10 +273,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -778,7 +780,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -792,7 +794,7 @@
     <col min="7" max="7" width="25.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.7265625" style="3" customWidth="1"/>
     <col min="11" max="11" width="25.90625" style="3" customWidth="1"/>
     <col min="12" max="27" width="18.6328125" style="3" customWidth="1"/>
     <col min="28" max="16384" width="14.453125" style="3"/>
@@ -931,7 +933,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="58" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -982,7 +984,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1033,7 +1035,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="68" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1084,7 +1086,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="42.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="56.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1137,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="53" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="68.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -30036,5 +30038,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes made to stakeholder analysis
</commit_message>
<xml_diff>
--- a/stakeholder analysis.xlsx
+++ b/stakeholder analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nourb\Documents\GitHub\ProjM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB6671-A7EA-44E8-87C5-601EC0AE258B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D744128-1BE7-4449-9B45-B153E2F83A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,7 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -277,12 +277,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -397,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -408,28 +402,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -780,7 +771,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -801,35 +792,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="42" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="1"/>
@@ -852,10 +843,10 @@
     <row r="2" spans="1:27" ht="28" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5"/>
@@ -883,37 +874,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="98" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="10" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="1"/>

</xml_diff>